<commit_message>
updated RF reopening guidance
</commit_message>
<xml_diff>
--- a/files/NIH COVID-19 Notice of Special Interest (NOSI)_6.5.20.xlsx
+++ b/files/NIH COVID-19 Notice of Special Interest (NOSI)_6.5.20.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livealbany.sharepoint.com/sites/research/ualbanyresearch/COkjf6g35o7/Shared Documents/HTML Messages (Campus Communication)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{39E6FDBE-35A2-414B-ADE5-9E3731316142}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{83120881-EA26-436A-A8D0-E4D9BEB14C1F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{48022702-4B25-4B2F-9445-B15897EC0066}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2996716E-F58D-4987-8BE7-32082A494CAB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="342">
   <si>
     <t>Keyword</t>
   </si>
@@ -250,6 +250,9 @@
     <t>Rolling thru. 03/30/2020</t>
   </si>
   <si>
+    <t>Contacts vary by IC. Please refer to the end of the NOSI.</t>
+  </si>
+  <si>
     <t>R21</t>
   </si>
   <si>
@@ -499,9 +502,6 @@
     <t>Rolling thru. 04/15/2021</t>
   </si>
   <si>
-    <t>Contacts vary by IC. Please refer to the end of the NOSI.</t>
-  </si>
-  <si>
     <t>Alcohol Consumption</t>
   </si>
   <si>
@@ -670,6 +670,60 @@
     <t xml:space="preserve">The project and budget periods must be within the currently approved project period for the existing parent award.   </t>
   </si>
   <si>
+    <t>Communication Disorders</t>
+  </si>
+  <si>
+    <t>Notice of Special Interest (NOSI): NIDCD is Interested in Supporting Research on the Impact of  COVID-19 on Mission Specific Sensory and Communication Disorders</t>
+  </si>
+  <si>
+    <t>R01, R21, R41/R42, R43/R44</t>
+  </si>
+  <si>
+    <t>National Institute on Deafness and Other Communication Disorders (NIDCD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The scope of the proposed project should determine the project period. The maximum project period is five years.  </t>
+  </si>
+  <si>
+    <t>$500,000 in direct costs in any year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bracie Watson, Jr. Ph.D.
+NIDCD/Division of Scientific Programs
+Telephone: 301-402-3458
+Email: watsonb@nidcd.nih.gov </t>
+  </si>
+  <si>
+    <t>Secondary Health Effects</t>
+  </si>
+  <si>
+    <t>Notice of Special Interest (NOSI): Digital Healthcare Interventions to Address the Secondary Health Effects Related to Social, Behavioral, and Economic Impact of COVID-19</t>
+  </si>
+  <si>
+    <t>NIMH, NEI, NHLBI, NIA, NIAAA, NICHD, NIDCD, NIDCR, NIDDK, NIDA, NINR, NIMHD, NCCIH, NCATS, SGMRO, ODP, OBSSR, ORWH</t>
+  </si>
+  <si>
+    <t>1 Year, 2 years with strong justification</t>
+  </si>
+  <si>
+    <t>$200,000 in direct costs</t>
+  </si>
+  <si>
+    <t>Adam Haim, Ph.D._x000D_
+National Institute of Mental Health (NIMH)_x000D_
+Telephone: 301-435-3593_x000D_
+Email: Haima@mail.nih.gov</t>
+  </si>
+  <si>
+    <t>Notice of Special Interest (NOSI): Competitive and Administrative Supplements for Community Interventions to Reduce the Impact of COVID-19 on Health Disparity and Other Vulnerable Populations</t>
+  </si>
+  <si>
+    <t>NIMHD, NEI, NHLBI, NIA, NIAAA, NICHD, NIDCD, NIDCR, NIDDK, NIDA, NIEHS, NIMH, NCCIH, NCATS, SGMRO, ODP, OBSSR, ORWH</t>
+  </si>
+  <si>
+    <t>$250,000 in direct costs per year</t>
+  </si>
+  <si>
     <t>Release_Date</t>
   </si>
   <si>
@@ -1175,6 +1229,14 @@
   </si>
   <si>
     <t>https://grants.nih.gov/grants/guide/notice-files/NOT-DE-20-022.html</t>
+  </si>
+  <si>
+    <t>Rolling thru.
+9/7/2022</t>
+  </si>
+  <si>
+    <t>Rolling thru.
+12/15/2020</t>
   </si>
 </sst>
 </file>
@@ -1339,7 +1401,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1363,9 +1425,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1723,18 +1782,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7865C998-A8E2-4648-AD75-66D19CA751FE}">
-  <dimension ref="A1:K46"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" style="22" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" style="21" customWidth="1"/>
     <col min="2" max="4" width="25.7109375" style="8" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="8" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" style="8" customWidth="1"/>
     <col min="6" max="6" width="17.140625" style="8" customWidth="1"/>
     <col min="7" max="7" width="23.42578125" style="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.5703125" style="8" customWidth="1"/>
@@ -1744,8 +1804,8 @@
     <col min="12" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:11" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1780,34 +1840,34 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="150" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="12" t="s">
         <v>20</v>
       </c>
       <c r="K2" s="4" t="s">
@@ -1815,34 +1875,34 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="180" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="G3" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="H3" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="18" t="s">
+      <c r="I3" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="18" t="s">
+      <c r="J3" s="17" t="s">
         <v>20</v>
       </c>
       <c r="K3" s="5" t="s">
@@ -1850,34 +1910,34 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="120" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="13" t="s">
+      <c r="J4" s="12" t="s">
         <v>20</v>
       </c>
       <c r="K4" s="4" t="s">
@@ -1885,674 +1945,674 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="120" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="H5" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="I5" s="18" t="s">
+      <c r="I5" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="18" t="s">
+      <c r="J5" s="17" t="s">
         <v>20</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>107</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="11" t="str">
+      <c r="B6" s="10" t="str">
         <f>HYPERLINK(Results!K2,Results!A2)</f>
         <v>Notice of Special Interest (NOSI): Data Driven Research on Coronavirus Disease 2019 (COVID-19) (R21)</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13" t="s">
+      <c r="D6" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="E6" s="12"/>
+      <c r="F6" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="13">
         <v>43999</v>
       </c>
-      <c r="I6" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="J6" s="13" t="s">
+      <c r="I6" s="12" t="s">
         <v>43</v>
       </c>
+      <c r="J6" s="12" t="s">
+        <v>44</v>
+      </c>
       <c r="K6" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="150" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" s="15" t="str">
+      <c r="A7" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="14" t="str">
         <f>HYPERLINK(Results!K3,Results!A3)</f>
         <v>Notice of Special Interest (NOSI): Availability of Urgent Award for Competitive Revisions to IDeA-CTR Awards to Address the Need for Documenting 2019 Novel Coronavirus Disease (COVID-19)-Related Patient Outcomes</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="F7" s="18" t="s">
+      <c r="E7" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="F7" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="19">
+      <c r="H7" s="18">
         <v>44000</v>
       </c>
-      <c r="I7" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="J7" s="18" t="s">
-        <v>48</v>
+      <c r="I7" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="J7" s="17" t="s">
+        <v>49</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="135" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8" s="11" t="str">
+      <c r="A8" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="10" t="str">
         <f>HYPERLINK(Results!K4,Results!A4)</f>
         <v>Notice of Special Interest (NOSI): Availability of Emergency Competitive Revisions for Research on Severe Acute Respiratory Syndrome Coronavirus 2 (SARS-CoV-2) and Coronavirus Disease 2019 (COVID-19)</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="F8" s="13" t="s">
+      <c r="D8" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="E8" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="I8" s="13" t="s">
+      <c r="H8" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="13" t="s">
-        <v>54</v>
+      <c r="J8" s="12" t="s">
+        <v>55</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="135" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" s="15" t="str">
+      <c r="A9" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="14" t="str">
         <f>HYPERLINK(Results!K5,Results!A5)</f>
         <v>Notice of Special Interest (NOSI):  Administrative Supplements to Existing NIH ECHO Cooperative Agreements (Admin Supp - Clinical Trial Not Allowed) for Coronavirus Disease 2019 (COVID-19)  related Research</v>
       </c>
-      <c r="C9" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="D9" s="17" t="s">
+      <c r="C9" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18" t="s">
+      <c r="D9" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="E9" s="17"/>
+      <c r="F9" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="G9" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="19">
+      <c r="H9" s="18">
         <v>44004</v>
       </c>
-      <c r="I9" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="J9" s="18"/>
+      <c r="I9" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="J9" s="17"/>
       <c r="K9" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="135" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="B10" s="11" t="str">
+      <c r="A10" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="10" t="str">
         <f>HYPERLINK(Results!K6,Results!A6)</f>
         <v>Notice of Special Interest (NOSI): National Cancer Institute Announcement regarding Availability of Competitive Revision SBIR/STTR Supplements on Coronavirus Disease 2019 (COVID-19)</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="F10" s="13" t="s">
+      <c r="D10" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="E10" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="I10" s="13" t="s">
+      <c r="H10" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="I10" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="13" t="s">
-        <v>65</v>
+      <c r="J10" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="150" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="B11" s="15" t="str">
+      <c r="A11" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="14" t="str">
         <f>HYPERLINK(Results!K7,Results!A7)</f>
         <v>Notice of Special Interest (NOSI): National Cancer Institute Announcement Regarding Availability of Urgent Competitive Revision and Administrative Supplements on Coronavirus Disease 2019 (COVID-19)</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="G11" s="19" t="s">
+      <c r="D11" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="I11" s="18" t="s">
+      <c r="H11" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="I11" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="18" t="s">
-        <v>54</v>
+      <c r="J11" s="17" t="s">
+        <v>55</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="315" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="B12" s="11" t="str">
+      <c r="A12" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="10" t="str">
         <f>HYPERLINK(Results!K10,Results!A10)</f>
         <v>Notice of Special Interest (NOSI): Availability of Emergency Competitive Revisions on Coronavirus Disease 2019 (COVID-19) for Currently Active NHLBI Phase I-III Clinical Trials</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="E12" s="13" t="s">
+      <c r="D12" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="E12" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="F12" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="H12" s="14" t="s">
+      <c r="G12" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="I12" s="13" t="s">
+      <c r="H12" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="I12" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J12" s="13" t="s">
-        <v>76</v>
+      <c r="J12" s="12" t="s">
+        <v>77</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="135" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="B13" s="15" t="str">
+      <c r="A13" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="14" t="str">
         <f>HYPERLINK(Results!K12,Results!A12)</f>
         <v>Notice of Special Interest (NOSI): Availability of Emergency Competitive Revision and Administrative Supplements on Biomedical Technologies for Coronavirus Disease 2019 (COVID-19)</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="E13" s="18" t="s">
+      <c r="D13" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="E13" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="F13" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="G13" s="19" t="s">
+      <c r="G13" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H13" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="I13" s="18" t="s">
+      <c r="H13" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="I13" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="J13" s="18" t="s">
-        <v>82</v>
+      <c r="J13" s="17" t="s">
+        <v>83</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="180" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
-      <c r="B14" s="11" t="str">
+      <c r="A14" s="19"/>
+      <c r="B14" s="10" t="str">
         <f>HYPERLINK(Results!K13,Results!A13)</f>
         <v>Notice of Special Interest (NOSI): Availability of Emergency Competitive Revisions and Administrative Supplements to Clinical and Translational Science Award (CTSA) Program Awards to Address 2019 Novel Coronavirus Disease (COVID-19) Public Health Needs</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="K14" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="E14" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="G14" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H14" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="I14" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="J14" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>83</v>
-      </c>
     </row>
     <row r="15" spans="1:11" ht="105" x14ac:dyDescent="0.25">
-      <c r="A15" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="B15" s="15" t="str">
+      <c r="A15" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" s="14" t="str">
         <f>HYPERLINK(Results!K16,Results!A16)</f>
         <v>Notice of Special Interest (NOSI): Development of Biomedical Technologies for Coronavirus Disease 2019 (COVID-19)</v>
       </c>
-      <c r="C15" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="D15" s="17" t="s">
+      <c r="C15" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="I15" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="J15" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="E15" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="F15" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="G15" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="H15" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="I15" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="J15" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="K15" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="B16" s="11" t="str">
+      <c r="B16" s="10" t="str">
         <f>HYPERLINK(Results!K17,Results!A17)</f>
         <v>Notice of Special Interest (NOSI): Small Business Research and Development of Biomedical Technologies for Coronavirus Disease 2019 (COVID-19)</v>
       </c>
-      <c r="C16" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="E16" s="13" t="s">
+      <c r="C16" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="F16" s="13" t="s">
+      <c r="D16" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="G16" s="14" t="s">
+      <c r="F16" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="G16" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="H16" s="14" t="s">
+      <c r="H16" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="I16" s="13" t="s">
+      <c r="I16" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J16" s="13" t="s">
-        <v>95</v>
+      <c r="J16" s="12" t="s">
+        <v>96</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="135" x14ac:dyDescent="0.25">
-      <c r="A17" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="B17" s="15" t="str">
+      <c r="A17" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="B17" s="14" t="str">
         <f>HYPERLINK(Results!K19,Results!A19)</f>
         <v>Notice of Special Interest (NOSI): Availability of Urgent Competitive Revisions and Administrative Supplements For Research on Biological Effects of the 2019 Novel Coronavirus on the Nervous System</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="E17" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="F17" s="18" t="s">
+      <c r="D17" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="G17" s="19" t="s">
+      <c r="E17" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="G17" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H17" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="I17" s="18" t="s">
+      <c r="H17" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="I17" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="J17" s="18" t="s">
-        <v>82</v>
+      <c r="J17" s="17" t="s">
+        <v>83</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="225" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="B18" s="11" t="str">
+      <c r="A18" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="B18" s="10" t="str">
         <f>HYPERLINK(Results!K20,Results!A20)</f>
         <v>Notice of Special Interest (NOSI) regarding the Availability of Administrative Supplements and Urgent Competitive Revisions for Mental Health Research on the 2019 Novel Coronavirus</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="E18" s="13" t="s">
+      <c r="D18" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="F18" s="13" t="s">
+      <c r="E18" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="G18" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="H18" s="14" t="s">
+      <c r="F18" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="I18" s="13" t="s">
+      <c r="G18" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="H18" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="I18" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J18" s="13" t="s">
-        <v>82</v>
+      <c r="J18" s="12" t="s">
+        <v>83</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>107</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="135" x14ac:dyDescent="0.25">
-      <c r="A19" s="21" t="s">
+      <c r="A19" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="B19" s="15" t="str">
+      <c r="B19" s="14" t="str">
         <f>HYPERLINK(Results!K21,Results!A21)</f>
         <v>Notice of Special Interest:  Availability of Administrative Supplements and Competitive Revision Supplements on Coronavirus Disease 2019 (COVID-19) within the Mission of NIAAA</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="17" t="s">
+      <c r="D19" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="E19" s="18" t="s">
+      <c r="E19" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="18" t="s">
+      <c r="F19" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="G19" s="19" t="s">
+      <c r="G19" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H19" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="I19" s="18" t="s">
+      <c r="H19" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="I19" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="J19" s="18" t="s">
-        <v>82</v>
+      <c r="J19" s="17" t="s">
+        <v>83</v>
       </c>
       <c r="K19" s="5" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="120" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="B20" s="11" t="str">
+      <c r="B20" s="10" t="str">
         <f>HYPERLINK(Results!K22,Results!A22)</f>
         <v>Notice of Special Interest (NOSI): Competitive and Administrative Supplements for the Impact of COVID-19 Outbreak on Minority Health and Health Disparities</v>
       </c>
-      <c r="C20" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="D20" s="12" t="s">
+      <c r="C20" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="E20" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="F20" s="13" t="s">
+      <c r="E20" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="F20" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="G20" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="H20" s="14" t="s">
+      <c r="G20" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="H20" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="I20" s="13" t="s">
+      <c r="I20" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J20" s="13" t="s">
-        <v>82</v>
+      <c r="J20" s="12" t="s">
+        <v>83</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>107</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="105" x14ac:dyDescent="0.25">
-      <c r="A21" s="21" t="s">
+      <c r="A21" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="B21" s="15" t="str">
+      <c r="B21" s="14" t="str">
         <f>HYPERLINK(Results!K23,Results!A23)</f>
         <v>Notice of Special Interest (NOSI): NIA Availability of Administrative Supplements and Revision Supplements on Coronavirus Disease 2019 (COVID-19)</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="17" t="s">
+      <c r="D21" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="E21" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="F21" s="18" t="s">
+      <c r="E21" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="F21" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="G21" s="19" t="s">
+      <c r="G21" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H21" s="19" t="s">
+      <c r="H21" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="I21" s="18" t="s">
+      <c r="I21" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="J21" s="18" t="s">
+      <c r="J21" s="17" t="s">
         <v>119</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>107</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A22" s="20" t="s">
+      <c r="A22" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="B22" s="11" t="str">
+      <c r="B22" s="10" t="str">
         <f>HYPERLINK(Results!K24,Results!A24)</f>
         <v>Notice of Special Interest (NOSI): NIEHS Support for Understanding the Impact of Environmental Exposures on Coronavirus Disease 2019 (COVID-19)</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="E22" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="F22" s="13" t="s">
+      <c r="E22" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="F22" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="G22" s="14" t="s">
+      <c r="G22" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="H22" s="14" t="s">
+      <c r="H22" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="I22" s="13" t="s">
+      <c r="I22" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J22" s="13" t="s">
-        <v>82</v>
+      <c r="J22" s="12" t="s">
+        <v>83</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>107</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="225" x14ac:dyDescent="0.25">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="B23" s="15" t="str">
+      <c r="B23" s="14" t="str">
         <f>HYPERLINK(Results!K26,Results!A26)</f>
         <v>Notice of Special Interest (NOSI): Clinical and Translational Science Award (CTSA) Program Applications to Address 2019 Novel Coronavirus (COVID-19) Public Heath Need</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C23" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="D23" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="E23" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="F23" s="18" t="s">
+      <c r="D23" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="E23" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="G23" s="19" t="s">
+      <c r="F23" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="G23" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H23" s="19" t="s">
+      <c r="H23" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="I23" s="18" t="s">
+      <c r="I23" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="J23" s="18" t="s">
+      <c r="J23" s="17" t="s">
         <v>129</v>
       </c>
       <c r="K23" s="5" t="s">
@@ -2560,35 +2620,35 @@
       </c>
     </row>
     <row r="24" spans="1:11" ht="330" x14ac:dyDescent="0.25">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="B24" s="11" t="str">
+      <c r="B24" s="10" t="str">
         <f>HYPERLINK(Results!K27,Results!A27)</f>
         <v>Notice of Special Interest (NOSI): Select Research Areas for Severe Acute Respiratory Syndrome Coronavirus 2 (SARS-CoV-2) and Coronavirus Disease 2019 (COVID-19)</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D24" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="E24" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="F24" s="13" t="s">
+      <c r="E24" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="F24" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="G24" s="14" t="s">
+      <c r="G24" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="H24" s="14" t="s">
+      <c r="H24" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="I24" s="13" t="s">
+      <c r="I24" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J24" s="13" t="s">
+      <c r="J24" s="12" t="s">
         <v>136</v>
       </c>
       <c r="K24" s="4" t="s">
@@ -2596,141 +2656,141 @@
       </c>
     </row>
     <row r="25" spans="1:11" ht="105" x14ac:dyDescent="0.25">
-      <c r="A25" s="21" t="s">
+      <c r="A25" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="B25" s="15" t="str">
+      <c r="B25" s="14" t="str">
         <f>HYPERLINK(Results!K28,Results!A28)</f>
         <v>Notice of Special Interest (NOSI) regarding the Availability of Administrative Supplements for Tissue Chips Research on the 2019 Novel Coronavirus</v>
       </c>
-      <c r="C25" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="E25" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="F25" s="18" t="s">
+      <c r="C25" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F25" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="G25" s="19" t="s">
+      <c r="G25" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H25" s="19" t="s">
+      <c r="H25" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="I25" s="18" t="s">
+      <c r="I25" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="J25" s="18" t="s">
-        <v>82</v>
+      <c r="J25" s="17" t="s">
+        <v>83</v>
       </c>
       <c r="K25" s="5" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="135" x14ac:dyDescent="0.25">
-      <c r="A26" s="20" t="s">
+      <c r="A26" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="B26" s="11" t="str">
+      <c r="B26" s="10" t="str">
         <f>HYPERLINK(Results!K29,Results!A29)</f>
         <v>Notice of Special Interest (NOSI) regarding the Availability of Emergency Competitive Revisions to Existing NIH Grants and Cooperative Agreements for Tissue Chips Research on the 2019 Novel Coronavirus</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13" t="s">
+      <c r="D26" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="G26" s="14" t="s">
+      <c r="G26" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="H26" s="14" t="s">
+      <c r="H26" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="I26" s="13" t="s">
+      <c r="I26" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J26" s="13" t="s">
-        <v>82</v>
+      <c r="J26" s="12" t="s">
+        <v>83</v>
       </c>
       <c r="K26" s="4" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="150" x14ac:dyDescent="0.25">
-      <c r="A27" s="21" t="s">
+      <c r="A27" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="B27" s="15" t="str">
+      <c r="B27" s="14" t="str">
         <f>HYPERLINK(Results!K30,Results!A30)</f>
         <v>Notice of Special Interest (NOSI): Availability of Administrative Supplements and Urgent Competitive Revisions for Research on Stress Management in Relation to Coronavirus Disease 2019 (COVID-19)</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="17" t="s">
+      <c r="D27" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="E27" s="18" t="s">
+      <c r="E27" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="F27" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="G27" s="19" t="s">
+      <c r="F27" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="G27" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H27" s="19" t="s">
+      <c r="H27" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="I27" s="18" t="s">
+      <c r="I27" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="J27" s="18" t="s">
-        <v>82</v>
+      <c r="J27" s="17" t="s">
+        <v>83</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>107</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="240" x14ac:dyDescent="0.25">
-      <c r="A28" s="20" t="s">
+      <c r="A28" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="B28" s="11" t="str">
+      <c r="B28" s="10" t="str">
         <f>HYPERLINK(Results!K31,Results!A31)</f>
         <v>Notice of Special Interest (NOSI): Infrastructure Access for Research on Coronavirus Disease 2019 (COVID-19) Conducted in the National Dental Practice-Based Research Network</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="D28" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="E28" s="13" t="s">
+      <c r="E28" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="F28" s="13" t="s">
+      <c r="F28" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="G28" s="14" t="s">
+      <c r="G28" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="H28" s="14" t="s">
+      <c r="H28" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="I28" s="13" t="s">
+      <c r="I28" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J28" s="13" t="s">
+      <c r="J28" s="12" t="s">
         <v>136</v>
       </c>
       <c r="K28" s="4" t="s">
@@ -2738,92 +2798,279 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="225" x14ac:dyDescent="0.25">
-      <c r="A29" s="21" t="s">
+      <c r="A29" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="B29" s="15" t="str">
+      <c r="B29" s="14" t="str">
         <f>HYPERLINK(Results!K32,Results!A32)</f>
         <v>Notice of Special Interest (NOSI):? Availability of Urgent Competitive Revisions and Administrative Supplements for Coronavirus Disease 2019 (COVID-19) Research within the Mission of NIDCR</v>
       </c>
-      <c r="C29" s="16" t="s">
+      <c r="C29" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D29" s="17" t="s">
+      <c r="D29" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="E29" s="18" t="s">
+      <c r="E29" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="F29" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="G29" s="19" t="s">
+      <c r="F29" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="G29" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H29" s="19" t="s">
+      <c r="H29" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="I29" s="18" t="s">
+      <c r="I29" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="J29" s="18" t="s">
-        <v>82</v>
+      <c r="J29" s="17" t="s">
+        <v>83</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="10"/>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="10"/>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="10"/>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B38" s="10"/>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B39" s="10"/>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B40" s="10"/>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B41" s="10"/>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B42" s="10"/>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B43" s="10"/>
-    </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B44" s="10"/>
-    </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B45" s="10"/>
-    </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B46" s="10"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="195" x14ac:dyDescent="0.25">
+      <c r="A30" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="G30" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>340</v>
+      </c>
+      <c r="I30" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J30" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A31" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="F31" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="G31" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H31" s="18" t="s">
+        <v>341</v>
+      </c>
+      <c r="I31" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="J31" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="K31" s="5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+      <c r="A32" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="G32" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H32" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="I32" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J32" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="K32" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33"/>
+      <c r="B33"/>
+      <c r="C33"/>
+      <c r="D33"/>
+      <c r="E33"/>
+      <c r="F33"/>
+      <c r="G33"/>
+      <c r="H33"/>
+      <c r="I33"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34"/>
+      <c r="B34"/>
+      <c r="C34"/>
+      <c r="D34"/>
+      <c r="E34"/>
+      <c r="F34"/>
+      <c r="G34"/>
+      <c r="H34"/>
+      <c r="I34"/>
+      <c r="J34"/>
+      <c r="K34"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35"/>
+      <c r="B35"/>
+      <c r="C35"/>
+      <c r="D35"/>
+      <c r="E35"/>
+      <c r="F35"/>
+      <c r="G35"/>
+      <c r="H35"/>
+      <c r="I35"/>
+      <c r="J35"/>
+      <c r="K35"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36"/>
+      <c r="B36"/>
+      <c r="C36"/>
+      <c r="D36"/>
+      <c r="E36"/>
+      <c r="F36"/>
+      <c r="G36"/>
+      <c r="H36"/>
+      <c r="I36"/>
+      <c r="J36"/>
+      <c r="K36"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37"/>
+      <c r="B37"/>
+      <c r="C37"/>
+      <c r="D37"/>
+      <c r="E37"/>
+      <c r="F37"/>
+      <c r="G37"/>
+      <c r="H37"/>
+      <c r="I37"/>
+      <c r="J37"/>
+      <c r="K37"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38"/>
+      <c r="B38"/>
+      <c r="C38"/>
+      <c r="D38"/>
+      <c r="E38"/>
+      <c r="F38"/>
+      <c r="G38"/>
+      <c r="H38"/>
+      <c r="I38"/>
+      <c r="J38"/>
+      <c r="K38"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39"/>
+      <c r="B39"/>
+      <c r="C39"/>
+      <c r="D39"/>
+      <c r="E39"/>
+      <c r="F39"/>
+      <c r="G39"/>
+      <c r="H39"/>
+      <c r="I39"/>
+      <c r="J39"/>
+      <c r="K39"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40"/>
+      <c r="B40"/>
+      <c r="C40"/>
+      <c r="D40"/>
+      <c r="E40"/>
+      <c r="F40"/>
+      <c r="G40"/>
+      <c r="H40"/>
+      <c r="I40"/>
+      <c r="J40"/>
+      <c r="K40"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41"/>
+      <c r="B41"/>
+      <c r="C41"/>
+      <c r="D41"/>
+      <c r="E41"/>
+      <c r="F41"/>
+      <c r="G41"/>
+      <c r="H41"/>
+      <c r="I41"/>
+      <c r="J41"/>
+      <c r="K41"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K29" xr:uid="{9BBDD91C-2455-4B6D-9469-FE6B813A9214}"/>
+  <autoFilter ref="A1:K32" xr:uid="{9BBDD91C-2455-4B6D-9469-FE6B813A9214}"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{FA3C02C5-BC53-4E92-8C5B-911D30B9E6E3}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{D0C82610-6D60-47DD-8AE6-321E6436303A}"/>
     <hyperlink ref="B4" r:id="rId3" xr:uid="{82BED1FC-65D7-42F2-881E-CBCB94D63FA4}"/>
     <hyperlink ref="B5" r:id="rId4" xr:uid="{375C8826-D1CF-453A-933C-A4CA4AD4D757}"/>
+    <hyperlink ref="K30" r:id="rId5" xr:uid="{95FE95AF-A8F4-44A5-BD1E-53F1656D98B1}"/>
+    <hyperlink ref="K31" r:id="rId6" xr:uid="{81C0CF8B-F6BA-480E-A2B7-174078B8873C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId5"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId7"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A748FF8-A162-4F20-9926-894A8CAA02D2}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2846,244 +3093,244 @@
         <v>1</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>157</v>
+        <v>173</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>158</v>
+        <v>174</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>159</v>
+        <v>175</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>160</v>
+        <v>176</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>161</v>
+        <v>177</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>162</v>
+        <v>178</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>163</v>
+        <v>179</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>164</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>165</v>
+        <v>181</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>166</v>
+        <v>182</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>171</v>
+        <v>187</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>173</v>
+        <v>189</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>174</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>175</v>
+        <v>191</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>176</v>
+        <v>192</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>177</v>
+        <v>193</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>178</v>
+        <v>194</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>181</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>166</v>
-      </c>
       <c r="C4" s="6" t="s">
-        <v>183</v>
+        <v>199</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>184</v>
+        <v>200</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>185</v>
+        <v>201</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>186</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="I5" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>172</v>
-      </c>
       <c r="J5" s="6" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>191</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>192</v>
+        <v>208</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>193</v>
+        <v>209</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>194</v>
+        <v>210</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>195</v>
+        <v>211</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="H6" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="J6" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="I6" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>180</v>
-      </c>
       <c r="K6" s="6" t="s">
-        <v>197</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>198</v>
+        <v>214</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>193</v>
+        <v>209</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>194</v>
+        <v>210</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>195</v>
+        <v>211</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>199</v>
+        <v>215</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>200</v>
+        <v>216</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -3091,209 +3338,209 @@
         <v>23</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>201</v>
+        <v>217</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>202</v>
+        <v>218</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>204</v>
+        <v>220</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>205</v>
+        <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>206</v>
+        <v>222</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>207</v>
+        <v>223</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>208</v>
+        <v>224</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>209</v>
+        <v>225</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>210</v>
+        <v>226</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>211</v>
+        <v>227</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>212</v>
+        <v>228</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>166</v>
+        <v>182</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>208</v>
+        <v>224</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>209</v>
+        <v>225</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>213</v>
+        <v>229</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>214</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>215</v>
+        <v>231</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>216</v>
+        <v>232</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>217</v>
+        <v>233</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>218</v>
+        <v>234</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>219</v>
+        <v>235</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>220</v>
+        <v>236</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>221</v>
+        <v>237</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>222</v>
+        <v>238</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>223</v>
+        <v>239</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>224</v>
+        <v>240</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>225</v>
+        <v>241</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>226</v>
+        <v>242</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>227</v>
+        <v>243</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>228</v>
+        <v>244</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>229</v>
+        <v>245</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>230</v>
+        <v>246</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>219</v>
+        <v>235</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>231</v>
+        <v>247</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>232</v>
+        <v>248</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -3301,34 +3548,34 @@
         <v>30</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>233</v>
+        <v>249</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>234</v>
+        <v>250</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>178</v>
+        <v>194</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>235</v>
+        <v>251</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>236</v>
+        <v>252</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -3336,104 +3583,104 @@
         <v>36</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>237</v>
+        <v>253</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>238</v>
+        <v>254</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>239</v>
+        <v>255</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>240</v>
+        <v>256</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>241</v>
+        <v>257</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>242</v>
+        <v>258</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>223</v>
+        <v>239</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>238</v>
+        <v>254</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>225</v>
+        <v>241</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>243</v>
+        <v>259</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>244</v>
+        <v>260</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>245</v>
+        <v>261</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>223</v>
+        <v>239</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>238</v>
+        <v>254</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>225</v>
+        <v>241</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>246</v>
+        <v>262</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>247</v>
+        <v>263</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -3441,524 +3688,524 @@
         <v>12</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>248</v>
+        <v>264</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>249</v>
+        <v>265</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>250</v>
+        <v>266</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>251</v>
+        <v>267</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>252</v>
+        <v>268</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>253</v>
+        <v>269</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>254</v>
+        <v>270</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>255</v>
+        <v>271</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>256</v>
+        <v>272</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>257</v>
+        <v>273</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>258</v>
+        <v>274</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>259</v>
+        <v>275</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>260</v>
+        <v>276</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>193</v>
+        <v>209</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>261</v>
+        <v>277</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>262</v>
+        <v>278</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>263</v>
+        <v>279</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>264</v>
+        <v>280</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>265</v>
+        <v>281</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>266</v>
+        <v>282</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>267</v>
+        <v>283</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>261</v>
+        <v>277</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>268</v>
+        <v>284</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>270</v>
+        <v>286</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>271</v>
+        <v>287</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>193</v>
+        <v>209</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>272</v>
+        <v>288</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>273</v>
+        <v>289</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>274</v>
+        <v>290</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>275</v>
+        <v>291</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>276</v>
+        <v>292</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="B23" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="G23" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="C23" s="6" t="s">
-        <v>272</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>279</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>262</v>
-      </c>
       <c r="H23" s="6" t="s">
-        <v>280</v>
+        <v>296</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>281</v>
+        <v>297</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>282</v>
+        <v>298</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>223</v>
+        <v>239</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>283</v>
+        <v>299</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>121</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>284</v>
+        <v>300</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>285</v>
+        <v>301</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="K24" s="6" t="s">
-        <v>286</v>
+        <v>302</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>282</v>
+        <v>298</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>287</v>
+        <v>303</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>283</v>
+        <v>299</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>121</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>284</v>
+        <v>300</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>288</v>
+        <v>304</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="K25" s="6" t="s">
-        <v>289</v>
+        <v>305</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>290</v>
+        <v>306</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>291</v>
+        <v>307</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>292</v>
+        <v>308</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>127</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>219</v>
+        <v>235</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>293</v>
+        <v>309</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="K26" s="6" t="s">
-        <v>294</v>
+        <v>310</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>295</v>
+        <v>311</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>296</v>
+        <v>312</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>297</v>
+        <v>313</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>132</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>298</v>
+        <v>314</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>299</v>
+        <v>315</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>173</v>
+        <v>189</v>
       </c>
       <c r="K27" s="6" t="s">
-        <v>300</v>
+        <v>316</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>301</v>
+        <v>317</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>193</v>
+        <v>209</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>302</v>
+        <v>318</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>219</v>
+        <v>235</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>303</v>
+        <v>319</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="K28" s="6" t="s">
-        <v>304</v>
+        <v>320</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>305</v>
+        <v>321</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>193</v>
+        <v>209</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>302</v>
+        <v>318</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>219</v>
+        <v>235</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>306</v>
+        <v>322</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="K29" s="6" t="s">
-        <v>307</v>
+        <v>323</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>308</v>
+        <v>324</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>193</v>
+        <v>209</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>309</v>
+        <v>325</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>310</v>
+        <v>326</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>311</v>
+        <v>327</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>312</v>
+        <v>328</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>313</v>
+        <v>329</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>314</v>
+        <v>330</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>315</v>
+        <v>331</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>309</v>
+        <v>325</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>312</v>
+        <v>328</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>316</v>
+        <v>332</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>317</v>
+        <v>333</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>312</v>
+        <v>328</v>
       </c>
       <c r="K31" s="6" t="s">
-        <v>318</v>
+        <v>334</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>319</v>
+        <v>335</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>320</v>
+        <v>336</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>309</v>
+        <v>325</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>316</v>
+        <v>332</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>321</v>
+        <v>337</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>322</v>
+        <v>338</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="J32" s="6" t="s">
-        <v>312</v>
+        <v>328</v>
       </c>
       <c r="K32" s="7" t="s">
-        <v>323</v>
+        <v>339</v>
       </c>
     </row>
   </sheetData>
@@ -3976,6 +4223,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="20c30dde-31e7-480d-b1dd-7373eee4a6c2">
+      <UserInfo>
+        <DisplayName>Whitehouse, Kayla M</DisplayName>
+        <AccountId>1623</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010084A8BD5E599FD54D93F820ED6198B116" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="73e8845e775d9f2212d619f68696efe5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="20c30dde-31e7-480d-b1dd-7373eee4a6c2" xmlns:ns3="7aef31f0-4568-4676-8d14-d955c17f2274" xmlns:ns4="4F5EC4EF-EF70-4D01-B3E9-5E10636B4FB5" xmlns:ns5="4f5ec4ef-ef70-4d01-b3e9-5e10636b4fb5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a6abc86d85c9d5efc498eb81c3bf618c" ns2:_="" ns3:_="" ns4:_="" ns5:_="">
     <xsd:import namespace="20c30dde-31e7-480d-b1dd-7373eee4a6c2"/>
@@ -4216,12 +4477,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4232,6 +4487,25 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA2730CC-01FE-4C24-91D2-D251EC4191BE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="20c30dde-31e7-480d-b1dd-7373eee4a6c2"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7aef31f0-4568-4676-8d14-d955c17f2274"/>
+    <ds:schemaRef ds:uri="4F5EC4EF-EF70-4D01-B3E9-5E10636B4FB5"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="4f5ec4ef-ef70-4d01-b3e9-5e10636b4fb5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E3451C3-2F26-40A1-9F96-A9D46C03D94B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4252,25 +4526,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA2730CC-01FE-4C24-91D2-D251EC4191BE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="4f5ec4ef-ef70-4d01-b3e9-5e10636b4fb5"/>
-    <ds:schemaRef ds:uri="4F5EC4EF-EF70-4D01-B3E9-5E10636B4FB5"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="7aef31f0-4568-4676-8d14-d955c17f2274"/>
-    <ds:schemaRef ds:uri="20c30dde-31e7-480d-b1dd-7373eee4a6c2"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2751F155-2CF0-455D-AE42-476F405B7BEE}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Updated funding opps with logos
</commit_message>
<xml_diff>
--- a/files/NIH COVID-19 Notice of Special Interest (NOSI)_6.5.20.xlsx
+++ b/files/NIH COVID-19 Notice of Special Interest (NOSI)_6.5.20.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livealbany.sharepoint.com/sites/research/ualbanyresearch/COkjf6g35o7/Shared Documents/HTML Messages (Campus Communication)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{48022702-4B25-4B2F-9445-B15897EC0066}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0CA369CF-F83F-417F-A059-EFCFDD79DE1E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2996716E-F58D-4987-8BE7-32082A494CAB}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Results!$A$1:$K$32</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$43</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="386">
   <si>
     <t>Keyword</t>
   </si>
@@ -236,18 +236,13 @@
     <t>Rolling thru. 02/05/2021</t>
   </si>
   <si>
-    <t>Daniel E. Janes, Ph.D.
-National Institute of General Medical Sciences (NIGMS)
-Email: daniel.janes@nih.gov</t>
-  </si>
-  <si>
     <t>Notice of Special Interest (NOSI) regarding the Availability of Administrative Supplements and Urgent Competitive Revisions for Research on the 2019 Novel Coronavirus</t>
   </si>
   <si>
     <t>National Institute on Drug Abuse (NIDA)</t>
   </si>
   <si>
-    <t>Rolling thru. 03/30/2020</t>
+    <t>Rolling thru. 03/31/2020</t>
   </si>
   <si>
     <t>Contacts vary by IC. Please refer to the end of the NOSI.</t>
@@ -412,7 +407,7 @@
     <t>1 year (2 years with strong justification)</t>
   </si>
   <si>
-    <t>Rolling thru. 11/09/2020</t>
+    <t>Rolling thru. 11/10/2020</t>
   </si>
   <si>
     <t>6-page Research Strategy</t>
@@ -427,16 +422,25 @@
     <t>No more than parent award (more allowed with strong justification)</t>
   </si>
   <si>
-    <t>Rolling thru. 11/10/2020</t>
-  </si>
-  <si>
     <t>R01,R21,R03</t>
   </si>
   <si>
-    <t>5 years</t>
-  </si>
-  <si>
-    <t>Rolling thru. 03/30/2021</t>
+    <t>R01: 5 years
+R21: 2 years
+R03: 2 years</t>
+  </si>
+  <si>
+    <t>R01: No Limit, generally $500K per year;
+R21: $275,000 for total direct costs, no more than $200,000 in any single year
+R03: $50K per year</t>
+  </si>
+  <si>
+    <t>R01: June 5, 2020
+R21: June 16, 2020
+R03: June 16, 2020</t>
+  </si>
+  <si>
+    <t>Standard Dates Applied</t>
   </si>
   <si>
     <t>When developing applications in response to this NOSI, all instructions in the SF424 (R&amp;R) Application Guide and in the target funding opportunity announcement used for submission must be followed</t>
@@ -451,11 +455,10 @@
     <t>1 year for Phase I and 2 years for Phase II</t>
   </si>
   <si>
-    <t>Total funding support (direct costs, indirect costs, fee) normally may not exceed $252,131 for Phase I awards and $1,680,879 for Phase II awards. NIH has received a waiver from SBA, as authorized by statute, to exceed these total award amount hard caps for specific topics. The current list of approved topics can be found at https://sbir.nih.gov/funding#omni-sbir. Navigate to the “Program Descriptions and Research Topics” document, Appendix A or the "2019 SBA approved topics list for budget waivers"._x000D_
-_x000D_
-Each participating component may also set their own budget limit (higher or lower than the above) in the “Limited Amount of Award Section” of their respective topics section. Applicants are strongly encouraged to contact program officials prior to submitting any application in excess of the hard caps listed above and early in the application planning process. In all cases, applicants should propose a budget that is reasonable and appropriate for completion of the research project._x000D_
-_x000D_
-Phase IIB budgets must be submitted in accordance with participating IC-specific budget limitations described in the current SBIR/STTR Program Descriptions and Research Topics of the NIH.</t>
+    <t>Total funding support (direct costs, indirect costs, fee) normally may not exceed $252,131 for Phase I awards and $1,680,879 for Phase II awards. For more information, please see https://grants.nih.gov/grants/guide/pa-files/pa-19-270.html#_Section_II._Award_1.</t>
+  </si>
+  <si>
+    <t>Standard Dates Prior to 03/31/2021</t>
   </si>
   <si>
     <t>When developing applications in response to this NOSI, all instructions in the SF424 (R&amp;R) Application Guideand in the target funding opportunity announcement (PA-19-270, PA-19-272, PA-18-631) must be followed</t>
@@ -540,7 +543,7 @@
     <t>$100,000 direct costs per year (Contact program official for higher budget)</t>
   </si>
   <si>
-    <t>follow the instructions for their submission option (SF424 (R&amp;R) Application Guide, eRA Commons Administrative Supplement User Guide or PHS 398 Application Guide, as appropriate)</t>
+    <t>Page Limits for the activity code of the parent award must be followed</t>
   </si>
   <si>
     <t>Environmental exposures</t>
@@ -558,7 +561,7 @@
     <t>30 days prior to due date</t>
   </si>
   <si>
-    <t>Rolling thru. 05/04/2021</t>
+    <t>One Due Date Per Month Prior to 05/04/2021</t>
   </si>
   <si>
     <t>Informatics, translating biomedical discoveries into clinical applications</t>
@@ -567,7 +570,7 @@
     <t>Admin Supp,U01,R21,U54</t>
   </si>
   <si>
-    <t>Rolling thru. 07/10/2021</t>
+    <t>Due dates vary by activity code. Please refer to NOSI.</t>
   </si>
   <si>
     <t>follow the instructions in the Application Guide (SF424 (R&amp;R) Application Guide, eRA Commons Administrative Supplement User Guide or PHS 398 Application Guide, as appropriate)</t>
@@ -585,10 +588,15 @@
     <t>National Institute of Allergy and Infectious Diseases (NIAID)</t>
   </si>
   <si>
-    <t>$50,000 in direct costs each year</t>
-  </si>
-  <si>
-    <t>Rolling thru. 09/07/2021</t>
+    <t>R03: 2 years
+SBIR/STTR: 1 year for Phase I and 2 years for Phase II</t>
+  </si>
+  <si>
+    <t>R03: $50,000 in direct costs each year
+SBIR/STTR: Total funding support (direct costs, indirect costs, fee) normally may not exceed $252,131 for Phase I awards and $1,680,879 for Phase II awards. For more information, please see https://grants.nih.gov/grants/guide/pa-files/pa-19-270.html#_Section_II._Award_1.</t>
+  </si>
+  <si>
+    <t>June 16, 2020 -  September 8, 2021</t>
   </si>
   <si>
     <t>follow the instructions in the Research (R) Instructions in the SF424 (R&amp;R) Application Guide</t>
@@ -617,7 +625,7 @@
     <t>no more than 25% total costs of the amount of the current parent award</t>
   </si>
   <si>
-    <t>Rolling thru. 01/26/2022</t>
+    <t>Rolling thru. 01/25/2022</t>
   </si>
   <si>
     <t>Danilo A. Tagle, Ph.D.
@@ -627,9 +635,6 @@
   </si>
   <si>
     <t>no more than the amount of the current parent award</t>
-  </si>
-  <si>
-    <t>Rolling thru. 01/25/2022</t>
   </si>
   <si>
     <t>Stress management</t>
@@ -682,10 +687,12 @@
     <t>National Institute on Deafness and Other Communication Disorders (NIDCD)</t>
   </si>
   <si>
-    <t xml:space="preserve">The scope of the proposed project should determine the project period. The maximum project period is five years.  </t>
-  </si>
-  <si>
-    <t>$500,000 in direct costs in any year</t>
+    <t>R01: 5 years
+R21: 2 years
+SBIR/STTR: 1 year for Phase I and 2 years for Phase II</t>
+  </si>
+  <si>
+    <t>October 5, 2020 - September 8, 2022</t>
   </si>
   <si>
     <t xml:space="preserve">Bracie Watson, Jr. Ph.D.
@@ -709,6 +716,10 @@
     <t>$200,000 in direct costs</t>
   </si>
   <si>
+    <t>Rolling thru.
+12/15/2020</t>
+  </si>
+  <si>
     <t>Adam Haim, Ph.D._x000D_
 National Institute of Mental Health (NIMH)_x000D_
 Telephone: 301-435-3593_x000D_
@@ -724,6 +735,101 @@
     <t>$250,000 in direct costs per year</t>
   </si>
   <si>
+    <t>Sensory and Communication Disorders</t>
+  </si>
+  <si>
+    <t>Notice of Special Interest (NOSI): NIDCD is Interested in Supporting Research on the Impact of COVID-19 on Mission Specific Sensory and Communication Disorders</t>
+  </si>
+  <si>
+    <t>NIDCD</t>
+  </si>
+  <si>
+    <t>Budget varies by Activity Code (Ranges from $275,000 for 2-year project to unlimited)</t>
+  </si>
+  <si>
+    <t>Bracie Watson, Jr. Ph.D._x000D_
+NIDCD/Division of Scientific Programs_x000D_
+Telephone: 301-402-3458_x000D_
+Email: watsonb@nidcd.nih.gov</t>
+  </si>
+  <si>
+    <t>Digital Health Interventions, Health Disparities</t>
+  </si>
+  <si>
+    <t>Notice of Intent to Publish a Funding Opportunity Announcement for Digital healthcare interventions to address the secondary health effects related to social, behavioral, and economic impact of COVID-19 (R01 - Clinical Trial Optional)</t>
+  </si>
+  <si>
+    <t>R01</t>
+  </si>
+  <si>
+    <t>NIMH, NEI, NIA, NIAAA, NICHD, NIDCD, NIDCR, NIDA, NINR, NCCIH, ODP, OBSSR</t>
+  </si>
+  <si>
+    <t>up to three years</t>
+  </si>
+  <si>
+    <t>$750,000 in direct costs per year</t>
+  </si>
+  <si>
+    <t>Adam Haim, Ph.D
+National Institute of Mental Health (NIMH)
+301-435-3593
+haima@mail.nih.gov</t>
+  </si>
+  <si>
+    <t>Mental Health, Data Collection</t>
+  </si>
+  <si>
+    <t>Notice Announcing the Availability of Common Data Elements for Research Related to the Public Health Emergency caused by Coronavirus Disease 2019 (COVID-19)</t>
+  </si>
+  <si>
+    <t>National Institute of Mental Health (NIMH)</t>
+  </si>
+  <si>
+    <t>Gregory K. Farber, Ph.D._x000D_
+National Institute of Mental Health_x000D_
+Telephone: 301-435-0778_x000D_
+Email: farberg@mail.nih.gov</t>
+  </si>
+  <si>
+    <t>Health Disparities, Community Interventions</t>
+  </si>
+  <si>
+    <t>Notice of Intent to Publish a Funding Opportunity Announcement for Community Interventions to Address the Consequences of the COVID-19 Pandemic for Health Disparity and Vulnerable Populations (R01- Clinical Trial Optional)</t>
+  </si>
+  <si>
+    <t>NIMHD, NIA, NICHD, NIDCD, NIDCR, NIDA, NIEHS, NIMH, NINR, NCCIH, ODP, OBSSR, ORWH</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>Estimated July 22, 2020</t>
+  </si>
+  <si>
+    <t>Notice of Intent to Publish Funding Opportunity Announcements for the RADx-UP Initiatives</t>
+  </si>
+  <si>
+    <t>Competitive Revisions, U24</t>
+  </si>
+  <si>
+    <t>Estimated July 2020</t>
+  </si>
+  <si>
+    <t>Office of the Director, National Institutes of Health (OD):_x000D_
+Anna E. Mazzucco, PhD_x000D_
+301-538-2823_x000D_
+anna.mazzucco@nih.gov_x000D_
+National Institute on Aging (NIA):_x000D_
+Jonathan W. King, Ph.D._x000D_
+301-496-3136_x000D_
+kingjo@nia.nih.gov_x000D_
+National Institute on Minority Health and Health Disparities (NIMHD):_x000D_
+Nadra Tyus, Dr. P.H., M.P.H._x000D_
+301-594-8065_x000D_
+nadra.tyus@nih.gov</t>
+  </si>
+  <si>
     <t>Release_Date</t>
   </si>
   <si>
@@ -1231,12 +1337,85 @@
     <t>https://grants.nih.gov/grants/guide/notice-files/NOT-DE-20-022.html</t>
   </si>
   <si>
-    <t>Rolling thru.
-9/7/2022</t>
-  </si>
-  <si>
-    <t>Rolling thru.
-12/15/2020</t>
+    <t>R01: No Limit, generally $500K per year;
+R21: $275,000 for total direct costs, no more than $200,000 in any single year
+SBIR/STTR: Total funding support (direct costs, indirect costs, fee) normally may not exceed $252,131 for Phase I awards and $1,680,879 for Phase II awards. For more information, please see https://grants.nih.gov/grants/guide/pa-files/pa-19-270.html#_Section_II._Award_1.</t>
+  </si>
+  <si>
+    <t>Estimated due date in July 2020</t>
+  </si>
+  <si>
+    <t>12-Page Research Strategy</t>
+  </si>
+  <si>
+    <t>Infrastructure/Data Access</t>
+  </si>
+  <si>
+    <t>Generally, 5 Years</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For U24, generally, 5 years </t>
+  </si>
+  <si>
+    <t>For U24, generally, application budgets are not limited but need to reflect the actual needs of the proposed project.</t>
+  </si>
+  <si>
+    <t>Generally, application budgets are not limited but need to reflect the actual needs of the proposed project.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Daniel E. Janes, Ph.D.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+National Institute of General Medical Sciences (NIGMS)
+Email: daniel.janes@nih.gov</t>
+    </r>
+  </si>
+  <si>
+    <t>COVID-19</t>
+  </si>
+  <si>
+    <t>Emergency Awards: Rapid Investigation of Severe Acute Respiratory Syndrome Coronavirus 2 (SARS-CoV-2) and Coronavirus Disease 2019 (COVID-19) (R01 Clinical Trial Not Allowed)</t>
+  </si>
+  <si>
+    <t>5 years</t>
+  </si>
+  <si>
+    <t>No Limit (although budget should reflect the actual needs); Special permission needed for over $500,000 direct costs a year</t>
+  </si>
+  <si>
+    <t>Rolling thru. 4/30/2021</t>
+  </si>
+  <si>
+    <t>https://grants.nih.gov/grants/guide/pa-files/PAR-20-178.html#_Section_VII._Agency</t>
+  </si>
+  <si>
+    <t>Emergency Awards: Rapid Investigation of Severe Acute Respiratory Syndrome Coronavirus 2 (SARS-CoV-2) and Coronavirus Disease 2019 (COVID-19) (R21 Clinical Trial Not Allowed)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$275,000 total for direct costs </t>
+  </si>
+  <si>
+    <t>https://grants.nih.gov/grants/guide/pa-files/PAR-20-177.html#_Section_VII._Agency</t>
+  </si>
+  <si>
+    <t>12-page Research Strategy</t>
   </si>
 </sst>
 </file>
@@ -1305,7 +1484,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1330,8 +1509,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1394,6 +1579,68 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1401,7 +1648,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1441,9 +1688,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1465,6 +1709,51 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1472,7 +1761,38 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{16376FB0-71D6-4B6E-AEED-9106C6FF04B5}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1783,7 +2103,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7865C998-A8E2-4648-AD75-66D19CA751FE}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1792,10 +2112,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" style="21" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" style="20" customWidth="1"/>
     <col min="2" max="4" width="25.7109375" style="8" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" style="8" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="34.140625" style="8" customWidth="1"/>
     <col min="7" max="7" width="23.42578125" style="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.5703125" style="8" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" style="8" customWidth="1"/>
@@ -1805,7 +2125,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1839,100 +2159,100 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="150" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+    <row r="2" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>376</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>377</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>180</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>134</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>378</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>379</v>
+      </c>
+      <c r="G2" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="34" t="s">
+        <v>380</v>
+      </c>
+      <c r="I2" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="33" t="s">
+        <v>385</v>
+      </c>
+      <c r="K2" s="35" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="24" t="s">
+        <v>376</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>382</v>
+      </c>
+      <c r="C3" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="36" t="s">
+        <v>134</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>383</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>380</v>
+      </c>
+      <c r="I3" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="K3" s="29" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E4" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F4" s="12" t="s">
         <v>16</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="180" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="120" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>33</v>
       </c>
       <c r="G4" s="13" t="s">
         <v>17</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="I4" s="12" t="s">
         <v>19</v>
@@ -1941,1091 +2261,1247 @@
         <v>20</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="120" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
-        <v>11</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>22</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="18" t="s">
+      <c r="I7" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="I5" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+    </row>
+    <row r="8" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="10" t="str">
+      <c r="B8" s="10" t="str">
         <f>HYPERLINK(Results!K2,Results!A2)</f>
         <v>Notice of Special Interest (NOSI): Data Driven Research on Coronavirus Disease 2019 (COVID-19) (R21)</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C8" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="E8" s="12"/>
+      <c r="F8" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12" t="s">
+      <c r="G8" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="13">
+        <v>43999</v>
+      </c>
+      <c r="I8" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="13">
-        <v>43999</v>
-      </c>
-      <c r="I6" s="12" t="s">
+      <c r="J8" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="J6" s="12" t="s">
+      <c r="K8" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K6" s="4" t="s">
+    </row>
+    <row r="9" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" ht="150" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7" s="14" t="str">
+      <c r="B9" s="14" t="str">
         <f>HYPERLINK(Results!K3,Results!A3)</f>
         <v>Notice of Special Interest (NOSI): Availability of Urgent Award for Competitive Revisions to IDeA-CTR Awards to Address the Need for Documenting 2019 Novel Coronavirus Disease (COVID-19)-Related Patient Outcomes</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C9" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D9" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E9" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="G9" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="17">
+        <v>44000</v>
+      </c>
+      <c r="I9" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="G7" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="18">
-        <v>44000</v>
-      </c>
-      <c r="I7" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="J7" s="17" t="s">
+      <c r="K9" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="K7" s="5" t="s">
+    </row>
+    <row r="10" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" ht="135" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" s="10" t="str">
+      <c r="B10" s="10" t="str">
         <f>HYPERLINK(Results!K4,Results!A4)</f>
         <v>Notice of Special Interest (NOSI): Availability of Emergency Competitive Revisions for Research on Severe Acute Respiratory Syndrome Coronavirus 2 (SARS-CoV-2) and Coronavirus Disease 2019 (COVID-19)</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C10" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D10" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="E8" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F8" s="12" t="s">
+      <c r="G10" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="G8" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="13" t="s">
+      <c r="I10" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="I8" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="J8" s="12" t="s">
+      <c r="K10" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="K8" s="4" t="s">
+    </row>
+    <row r="11" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+      <c r="A11" s="19" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" ht="135" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B9" s="14" t="str">
+      <c r="B11" s="14" t="str">
         <f>HYPERLINK(Results!K5,Results!A5)</f>
         <v>Notice of Special Interest (NOSI):  Administrative Supplements to Existing NIH ECHO Cooperative Agreements (Admin Supp - Clinical Trial Not Allowed) for Coronavirus Disease 2019 (COVID-19)  related Research</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C11" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="E11" s="16"/>
+      <c r="F11" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17" t="s">
+      <c r="G11" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="17">
+        <v>44011</v>
+      </c>
+      <c r="I11" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="J11" s="16"/>
+      <c r="K11" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="G9" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" s="18">
-        <v>44004</v>
-      </c>
-      <c r="I9" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="J9" s="17"/>
-      <c r="K9" s="5" t="s">
+    </row>
+    <row r="12" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" ht="135" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="B10" s="10" t="str">
+      <c r="B12" s="10" t="str">
         <f>HYPERLINK(Results!K6,Results!A6)</f>
         <v>Notice of Special Interest (NOSI): National Cancer Institute Announcement regarding Availability of Competitive Revision SBIR/STTR Supplements on Coronavirus Disease 2019 (COVID-19)</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C12" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D12" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="E10" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" s="12" t="s">
+      <c r="G12" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="G10" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="13" t="s">
+      <c r="I12" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="I10" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="J10" s="12" t="s">
+      <c r="K12" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="K10" s="4" t="s">
+    </row>
+    <row r="13" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+      <c r="A13" s="19" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" ht="150" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="B11" s="14" t="str">
+      <c r="B13" s="14" t="str">
         <f>HYPERLINK(Results!K7,Results!A7)</f>
         <v>Notice of Special Interest (NOSI): National Cancer Institute Announcement Regarding Availability of Urgent Competitive Revision and Administrative Supplements on Coronavirus Disease 2019 (COVID-19)</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C13" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" s="17" t="s">
+      <c r="D13" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="I13" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="K13" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="G11" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="H11" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="I11" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="J11" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="K11" s="5" t="s">
+    </row>
+    <row r="14" spans="1:11" ht="315" x14ac:dyDescent="0.25">
+      <c r="A14" s="18" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" ht="315" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="B12" s="10" t="str">
+      <c r="B14" s="10" t="str">
         <f>HYPERLINK(Results!K10,Results!A10)</f>
         <v>Notice of Special Interest (NOSI): Availability of Emergency Competitive Revisions on Coronavirus Disease 2019 (COVID-19) for Currently Active NHLBI Phase I-III Clinical Trials</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C14" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D14" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="F14" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="G14" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="H14" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="H12" s="13" t="s">
+      <c r="I14" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="I12" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="J12" s="12" t="s">
+      <c r="K14" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="K12" s="4" t="s">
+    </row>
+    <row r="15" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+      <c r="A15" s="19" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" ht="135" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="B13" s="14" t="str">
+      <c r="B15" s="14" t="str">
         <f>HYPERLINK(Results!K12,Results!A12)</f>
         <v>Notice of Special Interest (NOSI): Availability of Emergency Competitive Revision and Administrative Supplements on Biomedical Technologies for Coronavirus Disease 2019 (COVID-19)</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C15" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D15" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E15" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="F15" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="F13" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="G13" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="H13" s="18" t="s">
+      <c r="I15" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="J15" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="I13" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="J13" s="17" t="s">
+      <c r="K15" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K13" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="180" x14ac:dyDescent="0.25">
-      <c r="A14" s="19"/>
-      <c r="B14" s="10" t="str">
+    </row>
+    <row r="16" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+      <c r="A16" s="18"/>
+      <c r="B16" s="10" t="str">
         <f>HYPERLINK(Results!K13,Results!A13)</f>
         <v>Notice of Special Interest (NOSI): Availability of Emergency Competitive Revisions and Administrative Supplements to Clinical and Translational Science Award (CTSA) Program Awards to Address 2019 Novel Coronavirus Disease (COVID-19) Public Health Needs</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C16" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D16" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="F16" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="G16" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="F14" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="H14" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="I14" s="12" t="s">
+      <c r="I16" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J14" s="12" t="s">
+      <c r="J16" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="K16" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="K14" s="4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="105" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="B15" s="14" t="str">
+    </row>
+    <row r="17" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A17" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" s="14" t="str">
         <f>HYPERLINK(Results!K16,Results!A16)</f>
         <v>Notice of Special Interest (NOSI): Development of Biomedical Technologies for Coronavirus Disease 2019 (COVID-19)</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C17" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="F17" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="D15" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="E15" s="17" t="s">
+      <c r="G17" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="F15" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="G15" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="H15" s="18" t="s">
+      <c r="I17" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="I15" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="J15" s="17" t="s">
+      <c r="J17" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="K15" s="5" t="s">
+      <c r="K17" s="5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="B16" s="10" t="str">
+    <row r="18" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" s="10" t="str">
         <f>HYPERLINK(Results!K17,Results!A17)</f>
         <v>Notice of Special Interest (NOSI): Small Business Research and Development of Biomedical Technologies for Coronavirus Disease 2019 (COVID-19)</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C18" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="D16" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="E16" s="12" t="s">
+      <c r="D18" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E18" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F18" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="G16" s="13" t="s">
+      <c r="G18" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="H16" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I16" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="J16" s="12" t="s">
+      <c r="H18" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="K16" s="4" t="s">
+      <c r="I18" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="J18" s="12" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" ht="135" x14ac:dyDescent="0.25">
-      <c r="A17" s="20" t="s">
+      <c r="K18" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B17" s="14" t="str">
+    </row>
+    <row r="19" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+      <c r="A19" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="B19" s="14" t="str">
         <f>HYPERLINK(Results!K19,Results!A19)</f>
         <v>Notice of Special Interest (NOSI): Availability of Urgent Competitive Revisions and Administrative Supplements For Research on Biological Effects of the 2019 Novel Coronavirus on the Nervous System</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C19" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="E17" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="F17" s="17" t="s">
+      <c r="D19" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="G17" s="18" t="s">
+      <c r="E19" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="G19" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H17" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="I17" s="17" t="s">
+      <c r="H19" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="I19" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="J17" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="K17" s="5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="225" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
+      <c r="J19" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="K19" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B18" s="10" t="str">
+    </row>
+    <row r="20" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+      <c r="A20" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="B20" s="10" t="str">
         <f>HYPERLINK(Results!K20,Results!A20)</f>
         <v>Notice of Special Interest (NOSI) regarding the Availability of Administrative Supplements and Urgent Competitive Revisions for Mental Health Research on the 2019 Novel Coronavirus</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C20" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="E18" s="12" t="s">
+      <c r="D20" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="F18" s="12" t="s">
+      <c r="E20" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="G18" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="H18" s="13" t="s">
+      <c r="F20" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="I18" s="12" t="s">
+      <c r="G20" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="I20" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J18" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="K18" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="135" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="B19" s="14" t="str">
+      <c r="J20" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+      <c r="A21" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="B21" s="14" t="str">
         <f>HYPERLINK(Results!K21,Results!A21)</f>
         <v>Notice of Special Interest:  Availability of Administrative Supplements and Competitive Revision Supplements on Coronavirus Disease 2019 (COVID-19) within the Mission of NIAAA</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C21" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="E19" s="17" t="s">
+      <c r="D21" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="E21" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="G19" s="18" t="s">
+      <c r="F21" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="G21" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H19" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="I19" s="17" t="s">
+      <c r="H21" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="I21" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="J19" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="K19" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="120" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
+      <c r="J21" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="K21" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B20" s="10" t="str">
+    </row>
+    <row r="22" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="A22" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="B22" s="10" t="str">
         <f>HYPERLINK(Results!K22,Results!A22)</f>
         <v>Notice of Special Interest (NOSI): Competitive and Administrative Supplements for the Impact of COVID-19 Outbreak on Minority Health and Health Disparities</v>
       </c>
-      <c r="C20" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="F20" s="12" t="s">
+      <c r="C22" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="G20" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="H20" s="13" t="s">
+      <c r="E22" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="F22" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="I20" s="12" t="s">
+      <c r="G22" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="I22" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J20" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="K20" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="105" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="B21" s="14" t="str">
+      <c r="J22" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A23" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="B23" s="14" t="str">
         <f>HYPERLINK(Results!K23,Results!A23)</f>
         <v>Notice of Special Interest (NOSI): NIA Availability of Administrative Supplements and Revision Supplements on Coronavirus Disease 2019 (COVID-19)</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C23" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="E21" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="F21" s="17" t="s">
+      <c r="D23" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="G21" s="18" t="s">
+      <c r="E23" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="G23" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H21" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="I21" s="17" t="s">
+      <c r="H23" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="I23" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="J21" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="K21" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
+      <c r="J23" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="B22" s="10" t="str">
+      <c r="K23" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A24" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="B24" s="10" t="str">
         <f>HYPERLINK(Results!K24,Results!A24)</f>
         <v>Notice of Special Interest (NOSI): NIEHS Support for Understanding the Impact of Environmental Exposures on Coronavirus Disease 2019 (COVID-19)</v>
       </c>
-      <c r="C22" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="D22" s="11" t="s">
+      <c r="C24" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="E22" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="F22" s="12" t="s">
+      <c r="D24" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="G22" s="13" t="s">
+      <c r="E24" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="F24" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="H22" s="13" t="s">
+      <c r="G24" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="I22" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="J22" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="K22" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="225" x14ac:dyDescent="0.25">
-      <c r="A23" s="20" t="s">
+      <c r="H24" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="B23" s="14" t="str">
+      <c r="I24" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="J24" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+      <c r="A25" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="B25" s="14" t="str">
         <f>HYPERLINK(Results!K26,Results!A26)</f>
         <v>Notice of Special Interest (NOSI): Clinical and Translational Science Award (CTSA) Program Applications to Address 2019 Novel Coronavirus (COVID-19) Public Heath Need</v>
       </c>
-      <c r="C23" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="D23" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="E23" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="F23" s="17" t="s">
+      <c r="C25" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="E25" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="G23" s="18" t="s">
+      <c r="F25" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="G25" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H23" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="I23" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="J23" s="17" t="s">
+      <c r="H25" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="K23" s="5" t="s">
+      <c r="I25" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="J25" s="16" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" ht="330" x14ac:dyDescent="0.25">
-      <c r="A24" s="19" t="s">
+      <c r="K25" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="B24" s="10" t="str">
+    </row>
+    <row r="26" spans="1:11" ht="254.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="B26" s="10" t="str">
         <f>HYPERLINK(Results!K27,Results!A27)</f>
         <v>Notice of Special Interest (NOSI): Select Research Areas for Severe Acute Respiratory Syndrome Coronavirus 2 (SARS-CoV-2) and Coronavirus Disease 2019 (COVID-19)</v>
       </c>
-      <c r="C24" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="D24" s="11" t="s">
+      <c r="C26" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="E24" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="F24" s="12" t="s">
+      <c r="D26" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="G24" s="13" t="s">
+      <c r="E26" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="G26" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="H24" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="I24" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="J24" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="K24" s="4" t="s">
+      <c r="H26" s="13" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" ht="105" x14ac:dyDescent="0.25">
-      <c r="A25" s="20" t="s">
+      <c r="I26" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="J26" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="B25" s="14" t="str">
+      <c r="K26" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A27" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B27" s="14" t="str">
         <f>HYPERLINK(Results!K28,Results!A28)</f>
         <v>Notice of Special Interest (NOSI) regarding the Availability of Administrative Supplements for Tissue Chips Research on the 2019 Novel Coronavirus</v>
       </c>
-      <c r="C25" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="D25" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="E25" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="F25" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="G25" s="18" t="s">
+      <c r="C27" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="F27" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="G27" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H25" s="18" t="s">
+      <c r="H27" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="I27" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="J27" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="K27" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+      <c r="A28" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="I25" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="J25" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="K25" s="5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="135" x14ac:dyDescent="0.25">
-      <c r="A26" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="B26" s="10" t="str">
+      <c r="B28" s="10" t="str">
         <f>HYPERLINK(Results!K29,Results!A29)</f>
         <v>Notice of Special Interest (NOSI) regarding the Availability of Emergency Competitive Revisions to Existing NIH Grants and Cooperative Agreements for Tissue Chips Research on the 2019 Novel Coronavirus</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C28" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12" t="s">
+      <c r="D28" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="G28" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H28" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="G26" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="H26" s="13" t="s">
+      <c r="I28" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J28" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="K28" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="I26" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="J26" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="K26" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="150" x14ac:dyDescent="0.25">
-      <c r="A27" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="B27" s="14" t="str">
+    </row>
+    <row r="29" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+      <c r="A29" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="B29" s="14" t="str">
         <f>HYPERLINK(Results!K30,Results!A30)</f>
         <v>Notice of Special Interest (NOSI): Availability of Administrative Supplements and Urgent Competitive Revisions for Research on Stress Management in Relation to Coronavirus Disease 2019 (COVID-19)</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C29" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="E27" s="17" t="s">
+      <c r="D29" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="E29" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="F27" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="G27" s="18" t="s">
+      <c r="F29" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="G29" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H27" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="I27" s="17" t="s">
+      <c r="H29" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="I29" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="J27" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="K27" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="240" x14ac:dyDescent="0.25">
-      <c r="A28" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="B28" s="10" t="str">
+      <c r="J29" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="K29" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="A30" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B30" s="10" t="str">
         <f>HYPERLINK(Results!K31,Results!A31)</f>
         <v>Notice of Special Interest (NOSI): Infrastructure Access for Research on Coronavirus Disease 2019 (COVID-19) Conducted in the National Dental Practice-Based Research Network</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C30" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="G30" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="I30" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J30" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+      <c r="A31" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="D28" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="E28" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F28" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="G28" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="H28" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="I28" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="J28" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="K28" s="4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="225" x14ac:dyDescent="0.25">
-      <c r="A29" s="20" t="s">
-        <v>147</v>
-      </c>
-      <c r="B29" s="14" t="str">
+      <c r="B31" s="14" t="str">
         <f>HYPERLINK(Results!K32,Results!A32)</f>
         <v>Notice of Special Interest (NOSI):? Availability of Urgent Competitive Revisions and Administrative Supplements for Coronavirus Disease 2019 (COVID-19) Research within the Mission of NIDCR</v>
       </c>
-      <c r="C29" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D29" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="E29" s="17" t="s">
-        <v>154</v>
-      </c>
-      <c r="F29" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="G29" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="H29" s="18" t="s">
-        <v>151</v>
-      </c>
-      <c r="I29" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="J29" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="K29" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="195" x14ac:dyDescent="0.25">
-      <c r="A30" s="19" t="s">
-        <v>155</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="F30" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="G30" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="H30" s="13" t="s">
-        <v>340</v>
-      </c>
-      <c r="I30" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="J30" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="K30" s="4" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="105" x14ac:dyDescent="0.25">
-      <c r="A31" s="20" t="s">
-        <v>162</v>
-      </c>
-      <c r="B31" s="14" t="s">
-        <v>163</v>
-      </c>
       <c r="C31" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D31" s="16" t="s">
-        <v>164</v>
-      </c>
-      <c r="E31" s="17" t="s">
-        <v>165</v>
-      </c>
-      <c r="F31" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="G31" s="18" t="s">
+      <c r="D31" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="G31" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H31" s="18" t="s">
-        <v>341</v>
-      </c>
-      <c r="I31" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="J31" s="17" t="s">
-        <v>83</v>
+      <c r="H31" s="17">
+        <v>44137</v>
+      </c>
+      <c r="I31" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="J31" s="16" t="s">
+        <v>82</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="135" x14ac:dyDescent="0.25">
-      <c r="A32" s="19" t="s">
-        <v>112</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="210" x14ac:dyDescent="0.25">
+      <c r="A32" s="18" t="s">
+        <v>156</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>13</v>
+        <v>158</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>170</v>
+        <v>367</v>
       </c>
       <c r="G32" s="13" t="s">
         <v>17</v>
       </c>
       <c r="H32" s="13" t="s">
-        <v>341</v>
+        <v>161</v>
       </c>
       <c r="I32" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="J32" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="K32" s="4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A33" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="E33" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="F33" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="G33" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H33" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="I33" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="J32" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="K32" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33"/>
-      <c r="B33"/>
-      <c r="C33"/>
-      <c r="D33"/>
-      <c r="E33"/>
-      <c r="F33"/>
-      <c r="G33"/>
-      <c r="H33"/>
-      <c r="I33"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34"/>
-      <c r="B34"/>
-      <c r="C34"/>
-      <c r="D34"/>
-      <c r="E34"/>
-      <c r="F34"/>
-      <c r="G34"/>
-      <c r="H34"/>
-      <c r="I34"/>
-      <c r="J34"/>
-      <c r="K34"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35"/>
-      <c r="B35"/>
-      <c r="C35"/>
-      <c r="D35"/>
-      <c r="E35"/>
-      <c r="F35"/>
-      <c r="G35"/>
-      <c r="H35"/>
-      <c r="I35"/>
-      <c r="J35"/>
-      <c r="K35"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36"/>
-      <c r="B36"/>
-      <c r="C36"/>
-      <c r="D36"/>
-      <c r="E36"/>
-      <c r="F36"/>
-      <c r="G36"/>
-      <c r="H36"/>
-      <c r="I36"/>
-      <c r="J36"/>
-      <c r="K36"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37"/>
-      <c r="B37"/>
-      <c r="C37"/>
-      <c r="D37"/>
-      <c r="E37"/>
-      <c r="F37"/>
-      <c r="G37"/>
-      <c r="H37"/>
-      <c r="I37"/>
-      <c r="J37"/>
-      <c r="K37"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38"/>
-      <c r="B38"/>
-      <c r="C38"/>
-      <c r="D38"/>
-      <c r="E38"/>
-      <c r="F38"/>
-      <c r="G38"/>
-      <c r="H38"/>
-      <c r="I38"/>
-      <c r="J38"/>
-      <c r="K38"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39"/>
-      <c r="B39"/>
-      <c r="C39"/>
-      <c r="D39"/>
-      <c r="E39"/>
-      <c r="F39"/>
-      <c r="G39"/>
-      <c r="H39"/>
-      <c r="I39"/>
-      <c r="J39"/>
-      <c r="K39"/>
+      <c r="J33" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="K33" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+      <c r="A34" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="G34" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H34" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="I34" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J34" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="K34" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A35" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="E35" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="F35" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="G35" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H35" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="I35" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="J35" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="K35" s="23" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+      <c r="A36" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="G36" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H36" s="13" t="s">
+        <v>368</v>
+      </c>
+      <c r="I36" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="J36" s="12" t="s">
+        <v>369</v>
+      </c>
+      <c r="K36" s="4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A37" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>370</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="E37" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F37" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G37" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H37" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="I37" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="J37" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="K37" s="23" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="165" x14ac:dyDescent="0.25">
+      <c r="A38" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>371</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>374</v>
+      </c>
+      <c r="G38" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H38" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="I38" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="J38" s="12" t="s">
+        <v>369</v>
+      </c>
+      <c r="K38" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="B39" s="25" t="s">
+        <v>194</v>
+      </c>
+      <c r="C39" s="26" t="s">
+        <v>195</v>
+      </c>
+      <c r="D39" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="E39" s="27" t="s">
+        <v>372</v>
+      </c>
+      <c r="F39" s="27" t="s">
+        <v>373</v>
+      </c>
+      <c r="G39" s="28" t="s">
+        <v>192</v>
+      </c>
+      <c r="H39" s="28" t="s">
+        <v>196</v>
+      </c>
+      <c r="I39" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="J39" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="K39" s="29" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40"/>
@@ -3053,18 +3529,67 @@
       <c r="J41"/>
       <c r="K41"/>
     </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42"/>
+      <c r="B42"/>
+      <c r="C42"/>
+      <c r="D42"/>
+      <c r="E42"/>
+      <c r="F42"/>
+      <c r="G42"/>
+      <c r="H42"/>
+      <c r="I42"/>
+      <c r="J42"/>
+      <c r="K42"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43"/>
+      <c r="B43"/>
+      <c r="C43"/>
+      <c r="D43"/>
+      <c r="E43"/>
+      <c r="F43"/>
+      <c r="G43"/>
+      <c r="H43"/>
+      <c r="I43"/>
+      <c r="J43"/>
+      <c r="K43"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:K32" xr:uid="{9BBDD91C-2455-4B6D-9469-FE6B813A9214}"/>
+  <autoFilter ref="A1:K43" xr:uid="{167B332D-388E-497D-A502-9A12B2E36113}"/>
+  <conditionalFormatting sqref="B33:B1048576 B1 B4:B31">
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B32">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B3">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{FA3C02C5-BC53-4E92-8C5B-911D30B9E6E3}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{D0C82610-6D60-47DD-8AE6-321E6436303A}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{82BED1FC-65D7-42F2-881E-CBCB94D63FA4}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{375C8826-D1CF-453A-933C-A4CA4AD4D757}"/>
-    <hyperlink ref="K30" r:id="rId5" xr:uid="{95FE95AF-A8F4-44A5-BD1E-53F1656D98B1}"/>
-    <hyperlink ref="K31" r:id="rId6" xr:uid="{81C0CF8B-F6BA-480E-A2B7-174078B8873C}"/>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{FA3C02C5-BC53-4E92-8C5B-911D30B9E6E3}"/>
+    <hyperlink ref="B5" r:id="rId2" xr:uid="{D0C82610-6D60-47DD-8AE6-321E6436303A}"/>
+    <hyperlink ref="B6" r:id="rId3" xr:uid="{82BED1FC-65D7-42F2-881E-CBCB94D63FA4}"/>
+    <hyperlink ref="B7" r:id="rId4" xr:uid="{375C8826-D1CF-453A-933C-A4CA4AD4D757}"/>
+    <hyperlink ref="K32" r:id="rId5" xr:uid="{95FE95AF-A8F4-44A5-BD1E-53F1656D98B1}"/>
+    <hyperlink ref="K33" r:id="rId6" xr:uid="{81C0CF8B-F6BA-480E-A2B7-174078B8873C}"/>
+    <hyperlink ref="B35" r:id="rId7" xr:uid="{CF1DFA5F-ED50-406A-90D6-60C5C0697FD8}"/>
+    <hyperlink ref="B36" r:id="rId8" xr:uid="{6D536E23-D174-4CB0-B487-0311479510BF}"/>
+    <hyperlink ref="B37" r:id="rId9" xr:uid="{5117846A-3C33-40C9-A5FC-E2E405635A30}"/>
+    <hyperlink ref="B38" r:id="rId10" xr:uid="{8E2169FA-C51A-4F24-9A90-82CF8D3E5B7C}"/>
+    <hyperlink ref="B39" r:id="rId11" xr:uid="{2BB8BA11-80B0-43A4-95A1-D30F7A588F9E}"/>
+    <hyperlink ref="B32" r:id="rId12" xr:uid="{FCAAE474-57DC-4309-A876-B7BA475805B8}"/>
+    <hyperlink ref="B33" r:id="rId13" xr:uid="{339612F1-80BE-48DB-843C-05949D217AE9}"/>
+    <hyperlink ref="B34" r:id="rId14" xr:uid="{71D35E12-9510-46F8-B4D3-24801CB6BE78}"/>
+    <hyperlink ref="K35" r:id="rId15" xr:uid="{3B2BACB7-721B-4CC4-BE32-59F4A78A2E55}"/>
+    <hyperlink ref="K37" r:id="rId16" xr:uid="{528BAA02-A382-4DD1-8120-080A3AFD6B96}"/>
+    <hyperlink ref="B3" r:id="rId17" xr:uid="{C627B287-352E-4644-A145-415CD1289457}"/>
+    <hyperlink ref="B2" r:id="rId18" xr:uid="{C9858C7E-3D3B-4C04-B7D2-7CF1BE834DC7}"/>
+    <hyperlink ref="K2" r:id="rId19" location="_Section_VII._Agency" xr:uid="{17D899BA-AD43-4695-A1D6-AC91985A9238}"/>
+    <hyperlink ref="K3" r:id="rId20" location="_Section_VII._Agency" xr:uid="{936890E4-CFC4-41CB-A46E-EF597DB5ACC7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId7"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId21"/>
 </worksheet>
 </file>
 
@@ -3093,244 +3618,244 @@
         <v>1</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>171</v>
+        <v>198</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>172</v>
+        <v>199</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>173</v>
+        <v>200</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>174</v>
+        <v>201</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>175</v>
+        <v>202</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>176</v>
+        <v>203</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>177</v>
+        <v>204</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>178</v>
+        <v>205</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>179</v>
+        <v>206</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>180</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>181</v>
+        <v>208</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>182</v>
+        <v>209</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>183</v>
+        <v>210</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>184</v>
+        <v>211</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>185</v>
+        <v>212</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>186</v>
+        <v>213</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>187</v>
+        <v>214</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>188</v>
+        <v>215</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>189</v>
+        <v>216</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>190</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>191</v>
+        <v>218</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>192</v>
+        <v>219</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>193</v>
+        <v>220</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>194</v>
+        <v>221</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>185</v>
+        <v>212</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>186</v>
+        <v>213</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>195</v>
+        <v>222</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>188</v>
+        <v>215</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>196</v>
+        <v>223</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>197</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>198</v>
+        <v>225</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>182</v>
+        <v>209</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>199</v>
+        <v>226</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>200</v>
+        <v>227</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>185</v>
+        <v>212</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>186</v>
+        <v>213</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>201</v>
+        <v>228</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>188</v>
+        <v>215</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>196</v>
+        <v>223</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>202</v>
+        <v>229</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>203</v>
+        <v>230</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>204</v>
+        <v>231</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>205</v>
+        <v>232</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>185</v>
+        <v>212</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>185</v>
+        <v>212</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>186</v>
+        <v>213</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>206</v>
+        <v>233</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>188</v>
+        <v>215</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>196</v>
+        <v>223</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>207</v>
+        <v>234</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>208</v>
+        <v>235</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>209</v>
+        <v>236</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>210</v>
+        <v>237</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>211</v>
+        <v>238</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>185</v>
+        <v>212</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>186</v>
+        <v>213</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>212</v>
+        <v>239</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>188</v>
+        <v>215</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>196</v>
+        <v>223</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>213</v>
+        <v>240</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>214</v>
+        <v>241</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>209</v>
+        <v>236</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>210</v>
+        <v>237</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>211</v>
+        <v>238</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>185</v>
+        <v>212</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>186</v>
+        <v>213</v>
       </c>
       <c r="H7" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="I7" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="I7" s="6" t="s">
-        <v>188</v>
-      </c>
       <c r="J7" s="6" t="s">
-        <v>196</v>
+        <v>223</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>216</v>
+        <v>243</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -3338,209 +3863,209 @@
         <v>23</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>217</v>
+        <v>244</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>218</v>
+        <v>245</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>219</v>
+        <v>246</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>185</v>
+        <v>212</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>186</v>
+        <v>213</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>220</v>
+        <v>247</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>188</v>
+        <v>215</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>196</v>
+        <v>223</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>221</v>
+        <v>248</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>222</v>
+        <v>249</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="J9" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>196</v>
-      </c>
       <c r="K9" s="6" t="s">
-        <v>227</v>
+        <v>254</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>228</v>
+        <v>255</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>182</v>
+        <v>209</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>224</v>
+        <v>251</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>225</v>
+        <v>252</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>185</v>
+        <v>212</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>186</v>
+        <v>213</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>229</v>
+        <v>256</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>188</v>
+        <v>215</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>196</v>
+        <v>223</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>230</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>231</v>
+        <v>258</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>232</v>
+        <v>259</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>233</v>
+        <v>260</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>234</v>
+        <v>261</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>235</v>
+        <v>262</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>185</v>
+        <v>212</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>186</v>
+        <v>213</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>236</v>
+        <v>263</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>188</v>
+        <v>215</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>196</v>
+        <v>223</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>237</v>
+        <v>264</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>239</v>
+        <v>266</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>240</v>
+        <v>267</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>241</v>
+        <v>268</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>185</v>
+        <v>212</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>186</v>
+        <v>213</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>242</v>
+        <v>269</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>188</v>
+        <v>215</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>196</v>
+        <v>223</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>243</v>
+        <v>270</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>244</v>
+        <v>271</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>246</v>
+        <v>273</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>235</v>
+        <v>262</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>185</v>
+        <v>212</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>186</v>
+        <v>213</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>188</v>
+        <v>215</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>196</v>
+        <v>223</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>248</v>
+        <v>275</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -3548,139 +4073,139 @@
         <v>30</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>249</v>
+        <v>276</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>250</v>
+        <v>277</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>194</v>
+        <v>221</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>185</v>
+        <v>212</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>186</v>
+        <v>213</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>251</v>
+        <v>278</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>188</v>
+        <v>215</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>196</v>
+        <v>223</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>252</v>
+        <v>279</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>253</v>
+        <v>280</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>254</v>
+        <v>281</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>255</v>
+        <v>282</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>185</v>
+        <v>212</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>186</v>
+        <v>213</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>256</v>
+        <v>283</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>188</v>
+        <v>215</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>196</v>
+        <v>223</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>257</v>
+        <v>284</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>258</v>
+        <v>285</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>239</v>
+        <v>266</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>254</v>
+        <v>281</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>241</v>
+        <v>268</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>185</v>
+        <v>212</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>186</v>
+        <v>213</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>259</v>
+        <v>286</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>188</v>
+        <v>215</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>196</v>
+        <v>223</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>260</v>
+        <v>287</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>261</v>
+        <v>288</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>239</v>
+        <v>266</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>254</v>
+        <v>281</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>93</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>241</v>
+        <v>268</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>185</v>
+        <v>212</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>186</v>
+        <v>213</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>262</v>
+        <v>289</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>188</v>
+        <v>215</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>196</v>
+        <v>223</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>263</v>
+        <v>290</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -3688,524 +4213,524 @@
         <v>12</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>264</v>
+        <v>291</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>265</v>
+        <v>292</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>266</v>
+        <v>293</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>185</v>
+        <v>212</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>267</v>
+        <v>294</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>268</v>
+        <v>295</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>188</v>
+        <v>215</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>196</v>
+        <v>223</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>269</v>
+        <v>296</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>270</v>
+        <v>297</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>271</v>
+        <v>298</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>272</v>
+        <v>299</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>273</v>
+        <v>300</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>185</v>
+        <v>212</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>186</v>
+        <v>213</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>274</v>
+        <v>301</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>188</v>
+        <v>215</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>196</v>
+        <v>223</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>275</v>
+        <v>302</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>276</v>
+        <v>303</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>209</v>
+        <v>236</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>277</v>
+        <v>304</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>278</v>
+        <v>305</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>185</v>
+        <v>212</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>279</v>
+        <v>306</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>280</v>
+        <v>307</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>188</v>
+        <v>215</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>196</v>
+        <v>223</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>281</v>
+        <v>308</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>282</v>
+        <v>309</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>283</v>
+        <v>310</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>277</v>
+        <v>304</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>284</v>
+        <v>311</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>185</v>
+        <v>212</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>186</v>
+        <v>213</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>285</v>
+        <v>312</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>188</v>
+        <v>215</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>196</v>
+        <v>223</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>286</v>
+        <v>313</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>287</v>
+        <v>314</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>209</v>
+        <v>236</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>288</v>
+        <v>315</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>289</v>
+        <v>316</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>185</v>
+        <v>212</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>290</v>
+        <v>317</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>291</v>
+        <v>318</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>188</v>
+        <v>215</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>196</v>
+        <v>223</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>292</v>
+        <v>319</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>293</v>
+        <v>320</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>294</v>
+        <v>321</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>288</v>
+        <v>315</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>295</v>
+        <v>322</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>185</v>
+        <v>212</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>278</v>
+        <v>305</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>296</v>
+        <v>323</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>188</v>
+        <v>215</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>196</v>
+        <v>223</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>297</v>
+        <v>324</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>298</v>
+        <v>325</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>239</v>
+        <v>266</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>299</v>
+        <v>326</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>300</v>
+        <v>327</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>185</v>
+        <v>212</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>186</v>
+        <v>213</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>301</v>
+        <v>328</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>188</v>
+        <v>215</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>196</v>
+        <v>223</v>
       </c>
       <c r="K24" s="6" t="s">
-        <v>302</v>
+        <v>329</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>298</v>
+        <v>325</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>303</v>
+        <v>330</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>299</v>
+        <v>326</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>300</v>
+        <v>327</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>185</v>
+        <v>212</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>186</v>
+        <v>213</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>304</v>
+        <v>331</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>188</v>
+        <v>215</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>196</v>
+        <v>223</v>
       </c>
       <c r="K25" s="6" t="s">
-        <v>305</v>
+        <v>332</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>306</v>
+        <v>333</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>307</v>
+        <v>334</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>308</v>
+        <v>335</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>235</v>
+        <v>262</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>185</v>
+        <v>212</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>186</v>
+        <v>213</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>309</v>
+        <v>336</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>188</v>
+        <v>215</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>196</v>
+        <v>223</v>
       </c>
       <c r="K26" s="6" t="s">
-        <v>310</v>
+        <v>337</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>311</v>
+        <v>338</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>312</v>
+        <v>339</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>313</v>
+        <v>340</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>314</v>
+        <v>341</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>185</v>
+        <v>212</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>186</v>
+        <v>213</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>315</v>
+        <v>342</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>188</v>
+        <v>215</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>189</v>
+        <v>216</v>
       </c>
       <c r="K27" s="6" t="s">
-        <v>316</v>
+        <v>343</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>317</v>
+        <v>344</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>209</v>
+        <v>236</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>318</v>
+        <v>345</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>235</v>
+        <v>262</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>185</v>
+        <v>212</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>186</v>
+        <v>213</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>319</v>
+        <v>346</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>188</v>
+        <v>215</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>196</v>
+        <v>223</v>
       </c>
       <c r="K28" s="6" t="s">
-        <v>320</v>
+        <v>347</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>321</v>
+        <v>348</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>209</v>
+        <v>236</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>318</v>
+        <v>345</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>235</v>
+        <v>262</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>185</v>
+        <v>212</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>186</v>
+        <v>213</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>322</v>
+        <v>349</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>188</v>
+        <v>215</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>196</v>
+        <v>223</v>
       </c>
       <c r="K29" s="6" t="s">
-        <v>323</v>
+        <v>350</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>324</v>
+        <v>351</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>209</v>
+        <v>236</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>325</v>
+        <v>352</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>219</v>
+        <v>246</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>185</v>
+        <v>212</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>326</v>
+        <v>353</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>327</v>
+        <v>354</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>188</v>
+        <v>215</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>328</v>
+        <v>355</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>329</v>
+        <v>356</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>330</v>
+        <v>357</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>331</v>
+        <v>358</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>325</v>
+        <v>352</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>328</v>
+        <v>355</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>332</v>
+        <v>359</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>185</v>
+        <v>212</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>186</v>
+        <v>213</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>333</v>
+        <v>360</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>188</v>
+        <v>215</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>328</v>
+        <v>355</v>
       </c>
       <c r="K31" s="6" t="s">
-        <v>334</v>
+        <v>361</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>335</v>
+        <v>362</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>336</v>
+        <v>363</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>325</v>
+        <v>352</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>332</v>
+        <v>359</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>185</v>
+        <v>212</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>337</v>
+        <v>364</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>338</v>
+        <v>365</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>188</v>
+        <v>215</v>
       </c>
       <c r="J32" s="6" t="s">
-        <v>328</v>
+        <v>355</v>
       </c>
       <c r="K32" s="7" t="s">
-        <v>339</v>
+        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -4231,12 +4756,26 @@
         <AccountId>1623</AccountId>
         <AccountType/>
       </UserInfo>
+      <UserInfo>
+        <DisplayName>Delio, Vincent J</DisplayName>
+        <AccountId>35</AccountId>
+        <AccountType/>
+      </UserInfo>
     </SharedWithUsers>
   </documentManagement>
 </p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010084A8BD5E599FD54D93F820ED6198B116" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="73e8845e775d9f2212d619f68696efe5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="20c30dde-31e7-480d-b1dd-7373eee4a6c2" xmlns:ns3="7aef31f0-4568-4676-8d14-d955c17f2274" xmlns:ns4="4F5EC4EF-EF70-4D01-B3E9-5E10636B4FB5" xmlns:ns5="4f5ec4ef-ef70-4d01-b3e9-5e10636b4fb5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a6abc86d85c9d5efc498eb81c3bf618c" ns2:_="" ns3:_="" ns4:_="" ns5:_="">
     <xsd:import namespace="20c30dde-31e7-480d-b1dd-7373eee4a6c2"/>
@@ -4477,35 +5016,34 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA2730CC-01FE-4C24-91D2-D251EC4191BE}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="20c30dde-31e7-480d-b1dd-7373eee4a6c2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="4F5EC4EF-EF70-4D01-B3E9-5E10636B4FB5"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="4f5ec4ef-ef70-4d01-b3e9-5e10636b4fb5"/>
+    <ds:schemaRef ds:uri="7aef31f0-4568-4676-8d14-d955c17f2274"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="20c30dde-31e7-480d-b1dd-7373eee4a6c2"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7aef31f0-4568-4676-8d14-d955c17f2274"/>
-    <ds:schemaRef ds:uri="4F5EC4EF-EF70-4D01-B3E9-5E10636B4FB5"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="4f5ec4ef-ef70-4d01-b3e9-5e10636b4fb5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2751F155-2CF0-455D-AE42-476F405B7BEE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E3451C3-2F26-40A1-9F96-A9D46C03D94B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4524,12 +5062,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2751F155-2CF0-455D-AE42-476F405B7BEE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>